<commit_message>
Men and Women Category update
</commit_message>
<xml_diff>
--- a/Backend/hostel_data.xlsx
+++ b/Backend/hostel_data.xlsx
@@ -854,7 +854,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3">
@@ -864,7 +864,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4">
@@ -874,7 +874,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5">
@@ -884,7 +884,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6">
@@ -894,7 +894,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Men Page + Backend Updated
</commit_message>
<xml_diff>
--- a/Backend/hostel_data.xlsx
+++ b/Backend/hostel_data.xlsx
@@ -8,7 +8,8 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Students" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="final allocation" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="women allocation" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="men allocation" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
@@ -379,440 +380,620 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.66796875" defaultRowHeight="15.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="28.38" customWidth="1" style="6" min="1" max="1"/>
-    <col width="12.67" customWidth="1" style="6" min="2" max="9"/>
+    <col width="28.38" customWidth="1" style="6" min="1" max="2"/>
+    <col width="12.67" customWidth="1" style="6" min="3" max="11"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" s="7">
-      <c r="A1" s="8" t="inlineStr">
+      <c r="A1" s="6" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="B1" s="8" t="inlineStr">
         <is>
           <t>EMAIL</t>
         </is>
       </c>
-      <c r="B1" s="8" t="inlineStr">
+      <c r="C1" s="8" t="inlineStr">
         <is>
           <t>OLD ROOM</t>
         </is>
       </c>
-      <c r="C1" s="8" t="inlineStr">
+      <c r="D1" s="8" t="inlineStr">
         <is>
           <t>OLD HOSTEL</t>
         </is>
       </c>
-      <c r="D1" s="8" t="inlineStr">
+      <c r="E1" s="8" t="inlineStr">
+        <is>
+          <t>Old FLOOR</t>
+        </is>
+      </c>
+      <c r="F1" s="8" t="inlineStr">
         <is>
           <t>FLOOR1</t>
         </is>
       </c>
-      <c r="E1" s="8" t="inlineStr">
+      <c r="G1" s="8" t="inlineStr">
         <is>
           <t>PREF 1</t>
         </is>
       </c>
-      <c r="F1" s="8" t="inlineStr">
+      <c r="H1" s="8" t="inlineStr">
         <is>
           <t>FLOOR2</t>
         </is>
       </c>
-      <c r="G1" s="8" t="inlineStr">
+      <c r="I1" s="8" t="inlineStr">
         <is>
           <t>PREF 2</t>
         </is>
       </c>
-      <c r="H1" s="8" t="inlineStr">
+      <c r="J1" s="8" t="inlineStr">
         <is>
           <t>FLOOR3</t>
         </is>
       </c>
-      <c r="I1" s="8" t="inlineStr">
+      <c r="K1" s="8" t="inlineStr">
         <is>
           <t>PREF 3</t>
         </is>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" s="7">
-      <c r="A2" s="8" t="inlineStr">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>Women</t>
+        </is>
+      </c>
+      <c r="B2" s="8" t="inlineStr">
         <is>
           <t>112201035@smail.iitpkd.ac.in</t>
         </is>
       </c>
-      <c r="B2" s="8" t="n">
+      <c r="C2" s="8" t="n">
         <v>335</v>
       </c>
-      <c r="C2" s="8" t="inlineStr">
+      <c r="D2" s="8" t="inlineStr">
         <is>
           <t>Saveri Hostel</t>
         </is>
       </c>
-      <c r="D2" s="8" t="n">
-        <v>3</v>
-      </c>
       <c r="E2" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="G2" s="8" t="n">
         <v>335</v>
       </c>
-      <c r="F2" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="G2" s="8" t="inlineStr">
+      <c r="H2" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2" s="8" t="inlineStr">
         <is>
           <t>AF</t>
         </is>
       </c>
-      <c r="H2" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="I2" s="8" t="inlineStr">
+      <c r="J2" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="K2" s="8" t="inlineStr">
         <is>
           <t>MF</t>
         </is>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" s="7">
-      <c r="A3" s="8" t="inlineStr">
+      <c r="A3" s="6" t="inlineStr">
+        <is>
+          <t>Women</t>
+        </is>
+      </c>
+      <c r="B3" s="8" t="inlineStr">
         <is>
           <t>112201010@smail.iitpkd.ac.in</t>
         </is>
       </c>
-      <c r="B3" s="8" t="n">
+      <c r="C3" s="8" t="n">
         <v>301</v>
       </c>
-      <c r="C3" s="8" t="inlineStr">
+      <c r="D3" s="8" t="inlineStr">
         <is>
           <t>Saveri Hostel</t>
         </is>
       </c>
-      <c r="D3" s="8" t="n">
-        <v>3</v>
-      </c>
       <c r="E3" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="G3" s="8" t="n">
         <v>301</v>
       </c>
-      <c r="F3" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="G3" s="8" t="inlineStr">
+      <c r="H3" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" s="8" t="inlineStr">
         <is>
           <t>MF</t>
         </is>
       </c>
-      <c r="H3" s="8" t="n">
+      <c r="J3" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="I3" s="8" t="inlineStr">
+      <c r="K3" s="8" t="inlineStr">
         <is>
           <t>MF</t>
         </is>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1" s="7">
-      <c r="A4" s="8" t="inlineStr">
+      <c r="A4" s="6" t="inlineStr">
+        <is>
+          <t>Women</t>
+        </is>
+      </c>
+      <c r="B4" s="8" t="inlineStr">
         <is>
           <t>112201025@smail.iitpkd.ac.in</t>
         </is>
       </c>
-      <c r="B4" s="8" t="n">
+      <c r="C4" s="8" t="n">
         <v>301</v>
       </c>
-      <c r="C4" s="8" t="inlineStr">
+      <c r="D4" s="8" t="inlineStr">
         <is>
           <t>Saveri Hostel</t>
         </is>
       </c>
-      <c r="D4" s="8" t="n">
-        <v>3</v>
-      </c>
       <c r="E4" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" s="8" t="n">
         <v>301</v>
       </c>
-      <c r="F4" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="G4" s="8" t="inlineStr">
+      <c r="H4" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="I4" s="8" t="inlineStr">
         <is>
           <t>AF</t>
         </is>
       </c>
-      <c r="H4" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="I4" s="8" t="inlineStr">
+      <c r="J4" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="K4" s="8" t="inlineStr">
         <is>
           <t>MF</t>
         </is>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1" s="7">
-      <c r="A5" s="8" t="inlineStr">
+      <c r="A5" s="6" t="inlineStr">
+        <is>
+          <t>Women</t>
+        </is>
+      </c>
+      <c r="B5" s="8" t="inlineStr">
         <is>
           <t>112201015@smail.iitpkd.ac.in</t>
         </is>
       </c>
-      <c r="B5" s="8" t="n">
+      <c r="C5" s="8" t="n">
         <v>203</v>
       </c>
-      <c r="C5" s="8" t="inlineStr">
+      <c r="D5" s="8" t="inlineStr">
         <is>
           <t>Saveri Hostel</t>
         </is>
       </c>
-      <c r="D5" s="8" t="n">
+      <c r="E5" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="E5" s="8" t="inlineStr">
+      <c r="G5" s="8" t="inlineStr">
         <is>
           <t>MF</t>
         </is>
       </c>
-      <c r="F5" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="G5" s="8" t="n">
+      <c r="H5" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" s="8" t="n">
         <v>203</v>
       </c>
-      <c r="H5" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="I5" s="8" t="inlineStr">
+      <c r="J5" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="K5" s="8" t="inlineStr">
         <is>
           <t>AF</t>
         </is>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1" s="7">
-      <c r="A6" s="8" t="inlineStr">
+      <c r="A6" s="6" t="inlineStr">
+        <is>
+          <t>Women</t>
+        </is>
+      </c>
+      <c r="B6" s="8" t="inlineStr">
         <is>
           <t>112201030@smail.iitpkd.ac.in</t>
         </is>
       </c>
-      <c r="B6" s="8" t="n">
+      <c r="C6" s="8" t="n">
         <v>306</v>
       </c>
-      <c r="C6" s="8" t="inlineStr">
+      <c r="D6" s="8" t="inlineStr">
         <is>
           <t>Saveri Hostel</t>
         </is>
       </c>
-      <c r="D6" s="8" t="n">
+      <c r="E6" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="E6" s="8" t="inlineStr">
+      <c r="G6" s="8" t="inlineStr">
         <is>
           <t>AF</t>
         </is>
       </c>
-      <c r="F6" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="G6" s="8" t="inlineStr">
+      <c r="H6" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="I6" s="8" t="inlineStr">
         <is>
           <t>AF</t>
         </is>
       </c>
-      <c r="H6" s="8" t="n">
-        <v>3</v>
-      </c>
-      <c r="I6" s="8" t="inlineStr">
+      <c r="J6" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="K6" s="8" t="inlineStr">
         <is>
           <t>AF</t>
         </is>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1" s="7">
-      <c r="A7" s="9" t="n"/>
-      <c r="B7" s="9" t="n"/>
-      <c r="C7" s="9" t="n"/>
-      <c r="D7" s="9" t="n"/>
-      <c r="E7" s="9" t="n"/>
-      <c r="F7" s="9" t="n"/>
-      <c r="G7" s="10" t="n"/>
+      <c r="A7" s="6" t="inlineStr">
+        <is>
+          <t>Women</t>
+        </is>
+      </c>
+      <c r="B7" s="8" t="inlineStr">
+        <is>
+          <t>112201045@smail.iitpkd.ac.in</t>
+        </is>
+      </c>
+      <c r="C7" s="8" t="n">
+        <v>312</v>
+      </c>
+      <c r="D7" s="8" t="inlineStr">
+        <is>
+          <t>Saveri Hostel</t>
+        </is>
+      </c>
+      <c r="E7" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="8" t="inlineStr">
+        <is>
+          <t>AF</t>
+        </is>
+      </c>
+      <c r="H7" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" s="8" t="inlineStr">
+        <is>
+          <t>AF</t>
+        </is>
+      </c>
+      <c r="J7" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="K7" s="8" t="inlineStr">
+        <is>
+          <t>AF</t>
+        </is>
+      </c>
     </row>
     <row r="8" ht="15.75" customHeight="1" s="7">
-      <c r="A8" s="9" t="n"/>
-      <c r="B8" s="9" t="n"/>
-      <c r="C8" s="9" t="n"/>
-      <c r="D8" s="9" t="n"/>
-      <c r="E8" s="9" t="n"/>
-      <c r="F8" s="9" t="n"/>
-      <c r="G8" s="10" t="n"/>
+      <c r="A8" s="8" t="inlineStr">
+        <is>
+          <t>Men</t>
+        </is>
+      </c>
+      <c r="B8" s="8" t="inlineStr">
+        <is>
+          <t>112201035@smail.iitpkd.ac.in</t>
+        </is>
+      </c>
+      <c r="C8" s="8" t="n">
+        <v>335</v>
+      </c>
+      <c r="D8" s="8" t="inlineStr">
+        <is>
+          <t>Saveri Hostel</t>
+        </is>
+      </c>
+      <c r="E8" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="F8" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="G8" s="8" t="n">
+        <v>335</v>
+      </c>
+      <c r="H8" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="I8" s="8" t="inlineStr">
+        <is>
+          <t>MBS</t>
+        </is>
+      </c>
+      <c r="J8" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="K8" s="8" t="inlineStr">
+        <is>
+          <t>SMS</t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="15.75" customHeight="1" s="7">
-      <c r="A9" s="9" t="n"/>
-      <c r="B9" s="9" t="n"/>
-      <c r="C9" s="9" t="n"/>
-      <c r="D9" s="9" t="n"/>
-      <c r="E9" s="9" t="n"/>
-      <c r="F9" s="9" t="n"/>
-      <c r="G9" s="10" t="n"/>
+      <c r="A9" s="8" t="inlineStr">
+        <is>
+          <t>Men</t>
+        </is>
+      </c>
+      <c r="B9" s="8" t="inlineStr">
+        <is>
+          <t>112201035@smail.iitpkd.ac.in</t>
+        </is>
+      </c>
+      <c r="C9" s="8" t="n">
+        <v>325</v>
+      </c>
+      <c r="D9" s="8" t="inlineStr">
+        <is>
+          <t>Malhar Hostel</t>
+        </is>
+      </c>
+      <c r="E9" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="F9" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="G9" s="8" t="inlineStr">
+        <is>
+          <t>MF1S</t>
+        </is>
+      </c>
+      <c r="H9" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" s="8" t="inlineStr">
+        <is>
+          <t>MF1S</t>
+        </is>
+      </c>
+      <c r="J9" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" s="8" t="inlineStr">
+        <is>
+          <t>MF1S</t>
+        </is>
+      </c>
     </row>
     <row r="10" ht="15.75" customHeight="1" s="7">
-      <c r="A10" s="9" t="n"/>
       <c r="B10" s="9" t="n"/>
       <c r="C10" s="9" t="n"/>
       <c r="D10" s="9" t="n"/>
       <c r="E10" s="9" t="n"/>
       <c r="F10" s="9" t="n"/>
-      <c r="G10" s="10" t="n"/>
+      <c r="G10" s="9" t="n"/>
+      <c r="H10" s="9" t="n"/>
+      <c r="I10" s="10" t="n"/>
     </row>
     <row r="11" ht="15.75" customHeight="1" s="7">
-      <c r="A11" s="9" t="n"/>
       <c r="B11" s="9" t="n"/>
       <c r="C11" s="9" t="n"/>
       <c r="D11" s="9" t="n"/>
       <c r="E11" s="9" t="n"/>
       <c r="F11" s="9" t="n"/>
-      <c r="G11" s="10" t="n"/>
+      <c r="G11" s="9" t="n"/>
+      <c r="H11" s="9" t="n"/>
+      <c r="I11" s="10" t="n"/>
     </row>
     <row r="12" ht="15.75" customHeight="1" s="7">
-      <c r="A12" s="9" t="n"/>
       <c r="B12" s="9" t="n"/>
       <c r="C12" s="9" t="n"/>
       <c r="D12" s="9" t="n"/>
       <c r="E12" s="9" t="n"/>
       <c r="F12" s="9" t="n"/>
-      <c r="G12" s="10" t="n"/>
+      <c r="G12" s="9" t="n"/>
+      <c r="H12" s="9" t="n"/>
+      <c r="I12" s="10" t="n"/>
     </row>
     <row r="13" ht="15.75" customHeight="1" s="7">
-      <c r="A13" s="9" t="n"/>
       <c r="B13" s="9" t="n"/>
       <c r="C13" s="9" t="n"/>
       <c r="D13" s="9" t="n"/>
       <c r="E13" s="9" t="n"/>
       <c r="F13" s="9" t="n"/>
-      <c r="G13" s="10" t="n"/>
+      <c r="G13" s="9" t="n"/>
+      <c r="H13" s="9" t="n"/>
+      <c r="I13" s="10" t="n"/>
     </row>
     <row r="14" ht="15.75" customHeight="1" s="7">
-      <c r="A14" s="9" t="n"/>
       <c r="B14" s="9" t="n"/>
       <c r="C14" s="9" t="n"/>
       <c r="D14" s="9" t="n"/>
       <c r="E14" s="9" t="n"/>
       <c r="F14" s="9" t="n"/>
-      <c r="G14" s="10" t="n"/>
+      <c r="G14" s="9" t="n"/>
+      <c r="H14" s="9" t="n"/>
+      <c r="I14" s="10" t="n"/>
     </row>
     <row r="15" ht="15.75" customHeight="1" s="7">
-      <c r="A15" s="9" t="n"/>
       <c r="B15" s="9" t="n"/>
       <c r="C15" s="9" t="n"/>
       <c r="D15" s="9" t="n"/>
       <c r="E15" s="9" t="n"/>
       <c r="F15" s="9" t="n"/>
-      <c r="G15" s="10" t="n"/>
+      <c r="G15" s="9" t="n"/>
+      <c r="H15" s="9" t="n"/>
+      <c r="I15" s="10" t="n"/>
     </row>
     <row r="16" ht="15.75" customHeight="1" s="7">
-      <c r="A16" s="9" t="n"/>
       <c r="B16" s="9" t="n"/>
       <c r="C16" s="9" t="n"/>
       <c r="D16" s="9" t="n"/>
       <c r="E16" s="9" t="n"/>
       <c r="F16" s="9" t="n"/>
-      <c r="G16" s="10" t="n"/>
+      <c r="G16" s="9" t="n"/>
+      <c r="H16" s="9" t="n"/>
+      <c r="I16" s="10" t="n"/>
     </row>
     <row r="17" ht="15.75" customHeight="1" s="7">
-      <c r="A17" s="9" t="n"/>
       <c r="B17" s="9" t="n"/>
       <c r="C17" s="9" t="n"/>
       <c r="D17" s="9" t="n"/>
       <c r="E17" s="9" t="n"/>
       <c r="F17" s="9" t="n"/>
-      <c r="G17" s="10" t="n"/>
+      <c r="G17" s="9" t="n"/>
+      <c r="H17" s="9" t="n"/>
+      <c r="I17" s="10" t="n"/>
     </row>
     <row r="18" ht="15.75" customHeight="1" s="7">
-      <c r="A18" s="9" t="n"/>
       <c r="B18" s="9" t="n"/>
       <c r="C18" s="9" t="n"/>
       <c r="D18" s="9" t="n"/>
       <c r="E18" s="9" t="n"/>
       <c r="F18" s="9" t="n"/>
-      <c r="G18" s="10" t="n"/>
+      <c r="G18" s="9" t="n"/>
+      <c r="H18" s="9" t="n"/>
+      <c r="I18" s="10" t="n"/>
     </row>
     <row r="19" ht="15.75" customHeight="1" s="7">
-      <c r="A19" s="9" t="n"/>
       <c r="B19" s="9" t="n"/>
       <c r="C19" s="9" t="n"/>
       <c r="D19" s="9" t="n"/>
       <c r="E19" s="9" t="n"/>
       <c r="F19" s="9" t="n"/>
-      <c r="G19" s="10" t="n"/>
+      <c r="G19" s="9" t="n"/>
+      <c r="H19" s="9" t="n"/>
+      <c r="I19" s="10" t="n"/>
     </row>
     <row r="20" ht="15.75" customHeight="1" s="7">
-      <c r="A20" s="9" t="n"/>
       <c r="B20" s="9" t="n"/>
       <c r="C20" s="9" t="n"/>
       <c r="D20" s="9" t="n"/>
       <c r="E20" s="9" t="n"/>
       <c r="F20" s="9" t="n"/>
-      <c r="G20" s="10" t="n"/>
+      <c r="G20" s="9" t="n"/>
+      <c r="H20" s="9" t="n"/>
+      <c r="I20" s="10" t="n"/>
     </row>
     <row r="21" ht="15.75" customHeight="1" s="7">
-      <c r="A21" s="9" t="n"/>
       <c r="B21" s="9" t="n"/>
       <c r="C21" s="9" t="n"/>
       <c r="D21" s="9" t="n"/>
       <c r="E21" s="9" t="n"/>
       <c r="F21" s="9" t="n"/>
-      <c r="G21" s="10" t="n"/>
+      <c r="G21" s="9" t="n"/>
+      <c r="H21" s="9" t="n"/>
+      <c r="I21" s="10" t="n"/>
     </row>
     <row r="22" ht="15.75" customHeight="1" s="7">
-      <c r="A22" s="9" t="n"/>
       <c r="B22" s="9" t="n"/>
       <c r="C22" s="9" t="n"/>
       <c r="D22" s="9" t="n"/>
       <c r="E22" s="9" t="n"/>
       <c r="F22" s="9" t="n"/>
-      <c r="G22" s="10" t="n"/>
+      <c r="G22" s="9" t="n"/>
+      <c r="H22" s="9" t="n"/>
+      <c r="I22" s="10" t="n"/>
     </row>
     <row r="23" ht="15.75" customHeight="1" s="7">
-      <c r="A23" s="9" t="n"/>
       <c r="B23" s="9" t="n"/>
       <c r="C23" s="9" t="n"/>
       <c r="D23" s="9" t="n"/>
       <c r="E23" s="9" t="n"/>
       <c r="F23" s="9" t="n"/>
-      <c r="G23" s="10" t="n"/>
+      <c r="G23" s="9" t="n"/>
+      <c r="H23" s="9" t="n"/>
+      <c r="I23" s="10" t="n"/>
     </row>
     <row r="24" ht="15.75" customHeight="1" s="7">
-      <c r="A24" s="9" t="n"/>
       <c r="B24" s="9" t="n"/>
       <c r="C24" s="9" t="n"/>
       <c r="D24" s="9" t="n"/>
       <c r="E24" s="9" t="n"/>
       <c r="F24" s="9" t="n"/>
-      <c r="G24" s="10" t="n"/>
+      <c r="G24" s="9" t="n"/>
+      <c r="H24" s="9" t="n"/>
+      <c r="I24" s="10" t="n"/>
     </row>
     <row r="25" ht="15.75" customHeight="1" s="7">
-      <c r="A25" s="9" t="n"/>
       <c r="B25" s="9" t="n"/>
       <c r="C25" s="9" t="n"/>
       <c r="D25" s="9" t="n"/>
       <c r="E25" s="9" t="n"/>
       <c r="F25" s="9" t="n"/>
-      <c r="G25" s="10" t="n"/>
+      <c r="G25" s="9" t="n"/>
+      <c r="H25" s="9" t="n"/>
+      <c r="I25" s="10" t="n"/>
     </row>
     <row r="26" ht="15.75" customHeight="1" s="7">
-      <c r="A26" s="9" t="n"/>
       <c r="B26" s="9" t="n"/>
       <c r="C26" s="9" t="n"/>
       <c r="D26" s="9" t="n"/>
       <c r="E26" s="9" t="n"/>
       <c r="F26" s="9" t="n"/>
-      <c r="G26" s="10" t="n"/>
+      <c r="G26" s="9" t="n"/>
+      <c r="H26" s="9" t="n"/>
+      <c r="I26" s="10" t="n"/>
     </row>
     <row r="27" ht="15.75" customHeight="1" s="7">
-      <c r="A27" s="11" t="n"/>
       <c r="B27" s="11" t="n"/>
       <c r="C27" s="11" t="n"/>
       <c r="D27" s="11" t="n"/>
       <c r="E27" s="11" t="n"/>
       <c r="F27" s="11" t="n"/>
       <c r="G27" s="11" t="n"/>
+      <c r="H27" s="11" t="n"/>
+      <c r="I27" s="11" t="n"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
@@ -827,7 +1008,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -838,10 +1019,15 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>Gender</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>Email ID</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Allocated Room</t>
         </is>
@@ -850,51 +1036,157 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Women</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>112201035@smail.iitpkd.ac.in</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>223</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Women</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>112201010@smail.iitpkd.ac.in</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>202</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Women</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>112201025@smail.iitpkd.ac.in</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>222</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>Women</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>112201015@smail.iitpkd.ac.in</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>102</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>Women</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>112201030@smail.iitpkd.ac.in</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>126</v>
+      <c r="C6" t="n">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Women</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>112201045@smail.iitpkd.ac.in</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Gender</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Email ID</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Allocated Room</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Men</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>112201035@smail.iitpkd.ac.in</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Men</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>112201035@smail.iitpkd.ac.in</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>